<commit_message>
Implemented Registertest, NumpyninjaTest,PracticeQuestionsTest,RetryListnr, RetryAnalyzer
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DsAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DsAlgoTestData.xlsx
@@ -8,26 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0aa5a11d1390b959/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:801_{81E37865-FC61-42BF-8186-92FC58ACB5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EFD879A-C32B-4A75-9376-01D341919408}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:801_{81E37865-FC61-42BF-8186-92FC58ACB5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05B5E4DF-8917-427C-B1C3-6D02939211E9}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginUsernamePassword" sheetId="1" r:id="rId1"/>
     <sheet name="Arrays" sheetId="3" r:id="rId2"/>
-    <sheet name="DsAlgo" sheetId="2" r:id="rId3"/>
+    <sheet name="dstructure" sheetId="4" r:id="rId3"/>
+    <sheet name="DsAlgo" sheetId="2" r:id="rId4"/>
+    <sheet name="Pythoncode" sheetId="5" r:id="rId5"/>
+    <sheet name="PracticeQuestions" sheetId="6" r:id="rId6"/>
+    <sheet name="RegisterTest" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="j9wd9HEtPr1ocOaowijgj/jfgbWLpZCakALaVpRAbcc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="j9wd9HEtPr1ocOaowijgj/jfgbWLpZCakALaVpRAbcc="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -187,16 +191,170 @@
   <si>
     <t>Applications of Array</t>
   </si>
+  <si>
+    <t>timeComplexity</t>
+  </si>
+  <si>
+    <t>PythonCode</t>
+  </si>
+  <si>
+    <t>def search(list, value):
+    if value in list:
+        return "Element Found"
+    else:
+        return "Not Found"</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0
+    return max_count</t>
+  </si>
+  <si>
+    <t>def countEvenDigitNumbers(nums):
+    even_digit_count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            even_digit_count += 1
+    return even_digit_count</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    squared_nums = [x**2 for x in nums]
+    squared_nums.sort()
+    return squared_nums</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number of Digits</t>
+  </si>
+  <si>
+    <t>Squares of  a Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assessment</t>
+  </si>
+  <si>
+    <t>Pythoncode</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>question1</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>question3</t>
+  </si>
+  <si>
+    <t>question4</t>
+  </si>
+  <si>
+    <t>SucessMessage</t>
+  </si>
+  <si>
+    <t>FailedMessage</t>
+  </si>
+  <si>
+    <t>Some Tests failed. Please review code</t>
+  </si>
+  <si>
+    <t>def countNumbersWithEvenDigits(nums):
+    even_digit_count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            even_digit_count += 1
+    return even_digit_count</t>
+  </si>
+  <si>
+    <t>def search(input_list, value):       
+         if value in list:                                                                                     return "Element Found"
+    else:
+        return "Not Found"</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>No tests were collected</t>
+  </si>
+  <si>
+    <t>ValidationMessage</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Please fill out this field</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,6 +396,12 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,13 +423,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,6 +454,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1575,7 +1752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F558E89-049B-46E3-B588-CABF6663A4F3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1671,6 +1848,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F6B9DB-A520-444D-82F1-1F1F132F0F65}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1706,4 +1904,198 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F95D74C-4193-4750-876C-36B44594C41C}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="46.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="171" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="114" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0706CC9A-9311-4A48-AEEC-242653E41E5C}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="33.53125" customWidth="1"/>
+    <col min="2" max="2" width="21.1328125" customWidth="1"/>
+    <col min="3" max="3" width="46.265625" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="5" max="5" width="29.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="114.4" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9071BD-1337-4C1A-9888-F1FC85B06843}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>